<commit_message>
Fixed typo in FMAGX example
</commit_message>
<xml_diff>
--- a/Module 1/Week 2 - Fund structures and performance measures/FMAGX example.xlsx
+++ b/Module 1/Week 2 - Fund structures and performance measures/FMAGX example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Risk-free" sheetId="1" state="visible" r:id="rId2"/>
@@ -333,7 +333,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4385,11 +4385,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="34302861"/>
-        <c:axId val="55155570"/>
+        <c:axId val="22797826"/>
+        <c:axId val="85626654"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="34302861"/>
+        <c:axId val="22797826"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4417,7 +4417,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55155570"/>
+        <c:crossAx val="85626654"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4425,7 +4425,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55155570"/>
+        <c:axId val="85626654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4462,7 +4462,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34302861"/>
+        <c:crossAx val="22797826"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4510,7 +4510,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8568,11 +8568,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="18682114"/>
-        <c:axId val="65184128"/>
+        <c:axId val="31320012"/>
+        <c:axId val="6667835"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="18682114"/>
+        <c:axId val="31320012"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8600,7 +8600,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65184128"/>
+        <c:crossAx val="6667835"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8608,7 +8608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65184128"/>
+        <c:axId val="6667835"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8645,7 +8645,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18682114"/>
+        <c:crossAx val="31320012"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8704,9 +8704,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>75960</xdr:colOff>
+      <xdr:colOff>75240</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8714,8 +8714,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9310680" y="213480"/>
-        <a:ext cx="8961120" cy="5495760"/>
+        <a:off x="9314640" y="213480"/>
+        <a:ext cx="8988840" cy="5495040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8739,9 +8739,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>86400</xdr:colOff>
+      <xdr:colOff>85680</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>135720</xdr:rowOff>
+      <xdr:rowOff>135000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8749,8 +8749,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13033440" y="2248920"/>
-        <a:ext cx="10607760" cy="6649920"/>
+        <a:off x="13038840" y="2248920"/>
+        <a:ext cx="10631520" cy="6649200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8774,7 +8774,7 @@
       <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.91"/>
   </cols>
@@ -11398,10 +11398,10 @@
   <dimension ref="A1:F361"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P36" activeCellId="0" sqref="P36"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.08"/>
@@ -11436,6 +11436,7 @@
       <c r="C2" s="1" t="n">
         <v>0.045001</v>
       </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="5" t="n">
         <f aca="false">1+C2</f>
         <v>1.045001</v>
@@ -11455,6 +11456,7 @@
       <c r="C3" s="1" t="n">
         <v>0.071565</v>
       </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="5" t="n">
         <f aca="false">E2*(1+C3)</f>
         <v>1.119786496565</v>
@@ -11474,6 +11476,7 @@
       <c r="C4" s="1" t="n">
         <v>0.024355</v>
       </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="5" t="n">
         <f aca="false">E3*(1+C4)</f>
         <v>1.14705889668884</v>
@@ -11493,6 +11496,7 @@
       <c r="C5" s="1" t="n">
         <v>0.002268</v>
       </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="5" t="n">
         <f aca="false">E4*(1+C5)</f>
         <v>1.14966042626653</v>
@@ -11512,6 +11516,7 @@
       <c r="C6" s="1" t="n">
         <v>0.04293</v>
       </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="5" t="n">
         <f aca="false">E5*(1+C6)</f>
         <v>1.19901534836615</v>
@@ -11531,6 +11536,7 @@
       <c r="C7" s="1" t="n">
         <v>-0.045357</v>
       </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="5" t="n">
         <f aca="false">E6*(1+C7)</f>
         <v>1.14463160921031</v>
@@ -11550,6 +11556,7 @@
       <c r="C8" s="1" t="n">
         <v>0.046526</v>
       </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="5" t="n">
         <f aca="false">E7*(1+C8)</f>
         <v>1.19788673946043</v>
@@ -11569,6 +11576,7 @@
       <c r="C9" s="1" t="n">
         <v>0.023885</v>
       </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="5" t="n">
         <f aca="false">E8*(1+C9)</f>
         <v>1.22649826423244</v>
@@ -11588,6 +11596,7 @@
       <c r="C10" s="1" t="n">
         <v>-0.016861</v>
       </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="5" t="n">
         <f aca="false">E9*(1+C10)</f>
         <v>1.20581827699922</v>
@@ -11607,6 +11616,7 @@
       <c r="C11" s="1" t="n">
         <v>0.013458</v>
       </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="5" t="n">
         <f aca="false">E10*(1+C11)</f>
         <v>1.22204617937107</v>
@@ -11626,6 +11636,7 @@
       <c r="C12" s="1" t="n">
         <v>-0.040214</v>
       </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="5" t="n">
         <f aca="false">E11*(1+C12)</f>
         <v>1.17290281431384</v>
@@ -11645,6 +11656,7 @@
       <c r="C13" s="1" t="n">
         <v>0.114089</v>
       </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="5" t="n">
         <f aca="false">E12*(1+C13)</f>
         <v>1.3067181234961</v>
@@ -11664,6 +11676,7 @@
       <c r="C14" s="1" t="n">
         <v>-0.018348</v>
       </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="5" t="n">
         <f aca="false">E13*(1+C14)</f>
         <v>1.28274245936619</v>
@@ -11683,6 +11696,7 @@
       <c r="C15" s="1" t="n">
         <v>0.012865</v>
       </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="5" t="n">
         <f aca="false">E14*(1+C15)</f>
         <v>1.29924494110594</v>
@@ -11702,6 +11716,7 @@
       <c r="C16" s="1" t="n">
         <v>-0.01947</v>
       </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="5" t="n">
         <f aca="false">E15*(1+C16)</f>
         <v>1.2739486421026</v>
@@ -11721,6 +11736,7 @@
       <c r="C17" s="1" t="n">
         <v>0.028614</v>
       </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="5" t="n">
         <f aca="false">E16*(1+C17)</f>
         <v>1.31040140854773</v>
@@ -11740,6 +11756,7 @@
       <c r="C18" s="1" t="n">
         <v>0.00485</v>
       </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="5" t="n">
         <f aca="false">E17*(1+C18)</f>
         <v>1.31675685537918</v>
@@ -11759,6 +11776,7 @@
       <c r="C19" s="1" t="n">
         <v>-0.01503</v>
       </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="5" t="n">
         <f aca="false">E18*(1+C19)</f>
         <v>1.29696599984283</v>
@@ -11778,6 +11796,7 @@
       <c r="C20" s="1" t="n">
         <v>0.040924</v>
       </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="5" t="n">
         <f aca="false">E19*(1+C20)</f>
         <v>1.3500430364204</v>
@@ -11797,6 +11816,7 @@
       <c r="C21" s="1" t="n">
         <v>-0.020615</v>
       </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="5" t="n">
         <f aca="false">E20*(1+C21)</f>
         <v>1.3222118992246</v>
@@ -11816,6 +11836,7 @@
       <c r="C22" s="1" t="n">
         <v>0.01134</v>
       </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="5" t="n">
         <f aca="false">E21*(1+C22)</f>
         <v>1.3372057821618</v>
@@ -11835,6 +11856,7 @@
       <c r="C23" s="1" t="n">
         <v>0.004796</v>
       </c>
+      <c r="D23" s="1"/>
       <c r="E23" s="5" t="n">
         <f aca="false">E22*(1+C23)</f>
         <v>1.34361902109305</v>
@@ -11854,6 +11876,7 @@
       <c r="C24" s="1" t="n">
         <v>0.033794</v>
       </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="5" t="n">
         <f aca="false">E23*(1+C24)</f>
         <v>1.38902528229187</v>
@@ -11873,6 +11896,7 @@
       <c r="C25" s="1" t="n">
         <v>0.01338</v>
       </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="5" t="n">
         <f aca="false">E24*(1+C25)</f>
         <v>1.40761044056893</v>
@@ -11892,6 +11916,7 @@
       <c r="C26" s="1" t="n">
         <v>0.007282</v>
       </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="5" t="n">
         <f aca="false">E25*(1+C26)</f>
         <v>1.41786065979716</v>
@@ -11911,6 +11936,7 @@
       <c r="C27" s="1" t="n">
         <v>0.013526</v>
       </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="5" t="n">
         <f aca="false">E26*(1+C27)</f>
         <v>1.43703864308157</v>
@@ -11930,6 +11956,7 @@
       <c r="C28" s="1" t="n">
         <v>0.021202</v>
       </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="5" t="n">
         <f aca="false">E27*(1+C28)</f>
         <v>1.46750673639219</v>
@@ -11949,6 +11976,7 @@
       <c r="C29" s="1" t="n">
         <v>-0.024519</v>
       </c>
+      <c r="D29" s="1"/>
       <c r="E29" s="5" t="n">
         <f aca="false">E28*(1+C29)</f>
         <v>1.43152493872259</v>
@@ -11968,6 +11996,7 @@
       <c r="C30" s="1" t="n">
         <v>0.026259</v>
       </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="5" t="n">
         <f aca="false">E29*(1+C30)</f>
         <v>1.46911535208851</v>
@@ -11987,6 +12016,7 @@
       <c r="C31" s="1" t="n">
         <v>0.003466</v>
       </c>
+      <c r="D31" s="1"/>
       <c r="E31" s="5" t="n">
         <f aca="false">E30*(1+C31)</f>
         <v>1.47420730589884</v>
@@ -12006,6 +12036,7 @@
       <c r="C32" s="1" t="n">
         <v>-0.004593</v>
       </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="5" t="n">
         <f aca="false">E31*(1+C32)</f>
         <v>1.46743627174285</v>
@@ -12025,6 +12056,7 @@
       <c r="C33" s="1" t="n">
         <v>0.037431</v>
       </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="5" t="n">
         <f aca="false">E32*(1+C33)</f>
         <v>1.52236387883046</v>
@@ -12044,6 +12076,7 @@
       <c r="C34" s="1" t="n">
         <v>-0.007582</v>
       </c>
+      <c r="D34" s="1"/>
       <c r="E34" s="5" t="n">
         <f aca="false">E33*(1+C34)</f>
         <v>1.51082131590117</v>
@@ -12063,6 +12096,7 @@
       <c r="C35" s="1" t="n">
         <v>0.019884</v>
       </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="5" t="n">
         <f aca="false">E34*(1+C35)</f>
         <v>1.54086248694654</v>
@@ -12082,6 +12116,7 @@
       <c r="C36" s="1" t="n">
         <v>-0.008655</v>
       </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="5" t="n">
         <f aca="false">E35*(1+C36)</f>
         <v>1.52752632212202</v>
@@ -12101,6 +12136,7 @@
       <c r="C37" s="1" t="n">
         <v>0.012646</v>
       </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="5" t="n">
         <f aca="false">E36*(1+C37)</f>
         <v>1.54684341999158</v>
@@ -12120,6 +12156,7 @@
       <c r="C38" s="1" t="n">
         <v>0.033429</v>
       </c>
+      <c r="D38" s="1"/>
       <c r="E38" s="5" t="n">
         <f aca="false">E37*(1+C38)</f>
         <v>1.59855284867848</v>
@@ -12139,6 +12176,7 @@
       <c r="C39" s="1" t="n">
         <v>-0.027161</v>
       </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="5" t="n">
         <f aca="false">E38*(1+C39)</f>
         <v>1.55513455475552</v>
@@ -12158,6 +12196,7 @@
       <c r="C40" s="1" t="n">
         <v>-0.043456</v>
       </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="5" t="n">
         <f aca="false">E39*(1+C40)</f>
         <v>1.48755462754406</v>
@@ -12177,6 +12216,7 @@
       <c r="C41" s="1" t="n">
         <v>0.012817</v>
       </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="5" t="n">
         <f aca="false">E40*(1+C41)</f>
         <v>1.5066206152053</v>
@@ -12196,6 +12236,7 @@
       <c r="C42" s="1" t="n">
         <v>0.016309</v>
       </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="5" t="n">
         <f aca="false">E41*(1+C42)</f>
         <v>1.53119209081868</v>
@@ -12215,6 +12256,7 @@
       <c r="C43" s="1" t="n">
         <v>-0.024762</v>
       </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="5" t="n">
         <f aca="false">E42*(1+C43)</f>
         <v>1.49327671226583</v>
@@ -12234,6 +12276,7 @@
       <c r="C44" s="1" t="n">
         <v>0.032714</v>
       </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="5" t="n">
         <f aca="false">E43*(1+C44)</f>
         <v>1.54212776663089</v>
@@ -12253,6 +12296,7 @@
       <c r="C45" s="1" t="n">
         <v>0.041341</v>
       </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="5" t="n">
         <f aca="false">E44*(1+C45)</f>
         <v>1.60588087063118</v>
@@ -12272,6 +12316,7 @@
       <c r="C46" s="1" t="n">
         <v>-0.02394</v>
       </c>
+      <c r="D46" s="1"/>
       <c r="E46" s="5" t="n">
         <f aca="false">E45*(1+C46)</f>
         <v>1.56743608258827</v>
@@ -12291,6 +12336,7 @@
       <c r="C47" s="1" t="n">
         <v>0.022622</v>
       </c>
+      <c r="D47" s="1"/>
       <c r="E47" s="5" t="n">
         <f aca="false">E46*(1+C47)</f>
         <v>1.60289462164858</v>
@@ -12310,6 +12356,7 @@
       <c r="C48" s="1" t="n">
         <v>-0.036248</v>
       </c>
+      <c r="D48" s="1"/>
       <c r="E48" s="5" t="n">
         <f aca="false">E47*(1+C48)</f>
         <v>1.54479289740306</v>
@@ -12329,6 +12376,7 @@
       <c r="C49" s="1" t="n">
         <v>0.014955</v>
       </c>
+      <c r="D49" s="1"/>
       <c r="E49" s="5" t="n">
         <f aca="false">E48*(1+C49)</f>
         <v>1.56789527518373</v>
@@ -12348,6 +12396,7 @@
       <c r="C50" s="1" t="n">
         <v>0.026</v>
       </c>
+      <c r="D50" s="1"/>
       <c r="E50" s="5" t="n">
         <f aca="false">E49*(1+C50)</f>
         <v>1.6086605523385</v>
@@ -12367,6 +12416,7 @@
       <c r="C51" s="1" t="n">
         <v>0.039228</v>
       </c>
+      <c r="D51" s="1"/>
       <c r="E51" s="5" t="n">
         <f aca="false">E50*(1+C51)</f>
         <v>1.67176508848564</v>
@@ -12386,6 +12436,7 @@
       <c r="C52" s="1" t="n">
         <v>0.029334</v>
       </c>
+      <c r="D52" s="1"/>
       <c r="E52" s="5" t="n">
         <f aca="false">E51*(1+C52)</f>
         <v>1.72080464559127</v>
@@ -12405,6 +12456,7 @@
       <c r="C53" s="1" t="n">
         <v>0.029395</v>
       </c>
+      <c r="D53" s="1"/>
       <c r="E53" s="5" t="n">
         <f aca="false">E52*(1+C53)</f>
         <v>1.77138769814843</v>
@@ -12424,6 +12476,7 @@
       <c r="C54" s="1" t="n">
         <v>0.039809</v>
       </c>
+      <c r="D54" s="1"/>
       <c r="E54" s="5" t="n">
         <f aca="false">E53*(1+C54)</f>
         <v>1.84190487102402</v>
@@ -12443,6 +12496,7 @@
       <c r="C55" s="1" t="n">
         <v>0.024155</v>
       </c>
+      <c r="D55" s="1"/>
       <c r="E55" s="5" t="n">
         <f aca="false">E54*(1+C55)</f>
         <v>1.88639608318361</v>
@@ -12462,6 +12516,7 @@
       <c r="C56" s="1" t="n">
         <v>0.033405</v>
       </c>
+      <c r="D56" s="1"/>
       <c r="E56" s="5" t="n">
         <f aca="false">E55*(1+C56)</f>
         <v>1.94941114434235</v>
@@ -12481,6 +12536,7 @@
       <c r="C57" s="1" t="n">
         <v>0.003502</v>
       </c>
+      <c r="D57" s="1"/>
       <c r="E57" s="5" t="n">
         <f aca="false">E56*(1+C57)</f>
         <v>1.95623798216984</v>
@@ -12500,6 +12556,7 @@
       <c r="C58" s="1" t="n">
         <v>0.042102</v>
       </c>
+      <c r="D58" s="1"/>
       <c r="E58" s="5" t="n">
         <f aca="false">E57*(1+C58)</f>
         <v>2.03859951369516</v>
@@ -12519,6 +12576,7 @@
       <c r="C59" s="1" t="n">
         <v>-0.003442</v>
       </c>
+      <c r="D59" s="1"/>
       <c r="E59" s="5" t="n">
         <f aca="false">E58*(1+C59)</f>
         <v>2.03158265416902</v>
@@ -12538,6 +12596,7 @@
       <c r="C60" s="1" t="n">
         <v>0.044179</v>
       </c>
+      <c r="D60" s="1"/>
       <c r="E60" s="5" t="n">
         <f aca="false">E59*(1+C60)</f>
         <v>2.12133594424755</v>
@@ -12557,6 +12616,7 @@
       <c r="C61" s="1" t="n">
         <v>0.017643</v>
       </c>
+      <c r="D61" s="1"/>
       <c r="E61" s="5" t="n">
         <f aca="false">E60*(1+C61)</f>
         <v>2.15876267431191</v>
@@ -12576,6 +12636,7 @@
       <c r="C62" s="1" t="n">
         <v>0.034861</v>
       </c>
+      <c r="D62" s="1"/>
       <c r="E62" s="5" t="n">
         <f aca="false">E61*(1+C62)</f>
         <v>2.2340192999011</v>
@@ -12595,6 +12656,7 @@
       <c r="C63" s="1" t="n">
         <v>0.010088</v>
       </c>
+      <c r="D63" s="1"/>
       <c r="E63" s="5" t="n">
         <f aca="false">E62*(1+C63)</f>
         <v>2.2565560865985</v>
@@ -12614,6 +12676,7 @@
       <c r="C64" s="1" t="n">
         <v>0.009585</v>
       </c>
+      <c r="D64" s="1"/>
       <c r="E64" s="5" t="n">
         <f aca="false">E63*(1+C64)</f>
         <v>2.27818517668855</v>
@@ -12633,6 +12696,7 @@
       <c r="C65" s="1" t="n">
         <v>0.015133</v>
       </c>
+      <c r="D65" s="1"/>
       <c r="E65" s="5" t="n">
         <f aca="false">E64*(1+C65)</f>
         <v>2.31266095296737</v>
@@ -12652,6 +12716,7 @@
       <c r="C66" s="1" t="n">
         <v>0.025258</v>
       </c>
+      <c r="D66" s="1"/>
       <c r="E66" s="5" t="n">
         <f aca="false">E65*(1+C66)</f>
         <v>2.37107414331742</v>
@@ -12671,6 +12736,7 @@
       <c r="C67" s="1" t="n">
         <v>0.004128</v>
       </c>
+      <c r="D67" s="1"/>
       <c r="E67" s="5" t="n">
         <f aca="false">E66*(1+C67)</f>
         <v>2.38086193738104</v>
@@ -12690,6 +12756,7 @@
       <c r="C68" s="1" t="n">
         <v>-0.044444</v>
       </c>
+      <c r="D68" s="1"/>
       <c r="E68" s="5" t="n">
         <f aca="false">E67*(1+C68)</f>
         <v>2.27504690943608</v>
@@ -12709,6 +12776,7 @@
       <c r="C69" s="1" t="n">
         <v>0.021928</v>
       </c>
+      <c r="D69" s="1"/>
       <c r="E69" s="5" t="n">
         <f aca="false">E68*(1+C69)</f>
         <v>2.32493413806619</v>
@@ -12728,6 +12796,7 @@
       <c r="C70" s="1" t="n">
         <v>0.056035</v>
       </c>
+      <c r="D70" s="1"/>
       <c r="E70" s="5" t="n">
         <f aca="false">E69*(1+C70)</f>
         <v>2.45521182249273</v>
@@ -12747,6 +12816,7 @@
       <c r="C71" s="1" t="n">
         <v>0.026798</v>
       </c>
+      <c r="D71" s="1"/>
       <c r="E71" s="5" t="n">
         <f aca="false">E70*(1+C71)</f>
         <v>2.52100658891189</v>
@@ -12766,6 +12836,7 @@
       <c r="C72" s="1" t="n">
         <v>0.076441</v>
       </c>
+      <c r="D72" s="1"/>
       <c r="E72" s="5" t="n">
         <f aca="false">E71*(1+C72)</f>
         <v>2.7137148535749</v>
@@ -12785,6 +12856,7 @@
       <c r="C73" s="1" t="n">
         <v>-0.019798</v>
       </c>
+      <c r="D73" s="1"/>
       <c r="E73" s="5" t="n">
         <f aca="false">E72*(1+C73)</f>
         <v>2.65998872690383</v>
@@ -12804,6 +12876,7 @@
       <c r="C74" s="1" t="n">
         <v>0.062827</v>
       </c>
+      <c r="D74" s="1"/>
       <c r="E74" s="5" t="n">
         <f aca="false">E73*(1+C74)</f>
         <v>2.82710783864901</v>
@@ -12823,6 +12896,7 @@
       <c r="C75" s="1" t="n">
         <v>0.007752</v>
       </c>
+      <c r="D75" s="1"/>
       <c r="E75" s="5" t="n">
         <f aca="false">E74*(1+C75)</f>
         <v>2.84902357861422</v>
@@ -12842,6 +12916,7 @@
       <c r="C76" s="1" t="n">
         <v>-0.041688</v>
       </c>
+      <c r="D76" s="1"/>
       <c r="E76" s="5" t="n">
         <f aca="false">E75*(1+C76)</f>
         <v>2.73025348366895</v>
@@ -12861,6 +12936,7 @@
       <c r="C77" s="1" t="n">
         <v>0.060274</v>
       </c>
+      <c r="D77" s="1"/>
       <c r="E77" s="5" t="n">
         <f aca="false">E76*(1+C77)</f>
         <v>2.89481678214361</v>
@@ -12880,6 +12956,7 @@
       <c r="C78" s="1" t="n">
         <v>0.061401</v>
       </c>
+      <c r="D78" s="1"/>
       <c r="E78" s="5" t="n">
         <f aca="false">E77*(1+C78)</f>
         <v>3.07256142738401</v>
@@ -12899,6 +12976,7 @@
       <c r="C79" s="1" t="n">
         <v>0.044103</v>
       </c>
+      <c r="D79" s="1"/>
       <c r="E79" s="5" t="n">
         <f aca="false">E78*(1+C79)</f>
         <v>3.20807060401593</v>
@@ -12918,6 +12996,7 @@
       <c r="C80" s="1" t="n">
         <v>0.080388</v>
       </c>
+      <c r="D80" s="1"/>
       <c r="E80" s="5" t="n">
         <f aca="false">E79*(1+C80)</f>
         <v>3.46596098373156</v>
@@ -12937,6 +13016,7 @@
       <c r="C81" s="1" t="n">
         <v>-0.054975</v>
       </c>
+      <c r="D81" s="1"/>
       <c r="E81" s="5" t="n">
         <f aca="false">E80*(1+C81)</f>
         <v>3.27541977865092</v>
@@ -12956,6 +13036,7 @@
       <c r="C82" s="1" t="n">
         <v>0.053886</v>
       </c>
+      <c r="D82" s="1"/>
       <c r="E82" s="5" t="n">
         <f aca="false">E81*(1+C82)</f>
         <v>3.4519190488433</v>
@@ -12975,6 +13056,7 @@
       <c r="C83" s="1" t="n">
         <v>-0.032605</v>
       </c>
+      <c r="D83" s="1"/>
       <c r="E83" s="5" t="n">
         <f aca="false">E82*(1+C83)</f>
         <v>3.33936922825577</v>
@@ -12994,6 +13076,7 @@
       <c r="C84" s="1" t="n">
         <v>0.046321</v>
       </c>
+      <c r="D84" s="1"/>
       <c r="E84" s="5" t="n">
         <f aca="false">E83*(1+C84)</f>
         <v>3.4940521502778</v>
@@ -13013,6 +13096,7 @@
       <c r="C85" s="1" t="n">
         <v>0.017147</v>
       </c>
+      <c r="D85" s="1"/>
       <c r="E85" s="5" t="n">
         <f aca="false">E84*(1+C85)</f>
         <v>3.55396466249862</v>
@@ -13032,6 +13116,7 @@
       <c r="C86" s="1" t="n">
         <v>0.011994</v>
       </c>
+      <c r="D86" s="1"/>
       <c r="E86" s="5" t="n">
         <f aca="false">E85*(1+C86)</f>
         <v>3.59659091466063</v>
@@ -13051,6 +13136,7 @@
       <c r="C87" s="1" t="n">
         <v>0.071956</v>
       </c>
+      <c r="D87" s="1"/>
       <c r="E87" s="5" t="n">
         <f aca="false">E86*(1+C87)</f>
         <v>3.85538721051594</v>
@@ -13070,6 +13156,7 @@
       <c r="C88" s="1" t="n">
         <v>0.051336</v>
       </c>
+      <c r="D88" s="1"/>
       <c r="E88" s="5" t="n">
         <f aca="false">E87*(1+C88)</f>
         <v>4.05330736835499</v>
@@ -13089,6 +13176,7 @@
       <c r="C89" s="1" t="n">
         <v>0.011276</v>
       </c>
+      <c r="D89" s="1"/>
       <c r="E89" s="5" t="n">
         <f aca="false">E88*(1+C89)</f>
         <v>4.09901246224056</v>
@@ -13108,6 +13196,7 @@
       <c r="C90" s="1" t="n">
         <v>-0.017674</v>
       </c>
+      <c r="D90" s="1"/>
       <c r="E90" s="5" t="n">
         <f aca="false">E89*(1+C90)</f>
         <v>4.02656651598292</v>
@@ -13127,6 +13216,7 @@
       <c r="C91" s="1" t="n">
         <v>0.04097</v>
       </c>
+      <c r="D91" s="1"/>
       <c r="E91" s="5" t="n">
         <f aca="false">E90*(1+C91)</f>
         <v>4.19153494614274</v>
@@ -13146,6 +13236,7 @@
       <c r="C92" s="1" t="n">
         <v>-0.010109</v>
       </c>
+      <c r="D92" s="1"/>
       <c r="E92" s="5" t="n">
         <f aca="false">E91*(1+C92)</f>
         <v>4.14916271937219</v>
@@ -13165,6 +13256,7 @@
       <c r="C93" s="1" t="n">
         <v>-0.143124</v>
       </c>
+      <c r="D93" s="1"/>
       <c r="E93" s="5" t="n">
         <f aca="false">E92*(1+C93)</f>
         <v>3.55531795432476</v>
@@ -13184,6 +13276,7 @@
       <c r="C94" s="1" t="n">
         <v>0.063176</v>
       </c>
+      <c r="D94" s="1"/>
       <c r="E94" s="5" t="n">
         <f aca="false">E93*(1+C94)</f>
         <v>3.77992872140718</v>
@@ -13203,6 +13296,7 @@
       <c r="C95" s="1" t="n">
         <v>0.080111</v>
       </c>
+      <c r="D95" s="1"/>
       <c r="E95" s="5" t="n">
         <f aca="false">E94*(1+C95)</f>
         <v>4.08274259120783</v>
@@ -13222,6 +13316,7 @@
       <c r="C96" s="1" t="n">
         <v>0.062165</v>
       </c>
+      <c r="D96" s="1"/>
       <c r="E96" s="5" t="n">
         <f aca="false">E95*(1+C96)</f>
         <v>4.33654628439027</v>
@@ -13241,6 +13336,7 @@
       <c r="C97" s="1" t="n">
         <v>0.059673</v>
       </c>
+      <c r="D97" s="1"/>
       <c r="E97" s="5" t="n">
         <f aca="false">E96*(1+C97)</f>
         <v>4.59532101081869</v>
@@ -13260,6 +13356,7 @@
       <c r="C98" s="1" t="n">
         <v>0.0428</v>
       </c>
+      <c r="D98" s="1"/>
       <c r="E98" s="5" t="n">
         <f aca="false">E97*(1+C98)</f>
         <v>4.79200075008173</v>
@@ -13279,6 +13376,7 @@
       <c r="C99" s="1" t="n">
         <v>-0.031935</v>
       </c>
+      <c r="D99" s="1"/>
       <c r="E99" s="5" t="n">
         <f aca="false">E98*(1+C99)</f>
         <v>4.63896820612787</v>
@@ -13298,6 +13396,7 @@
       <c r="C100" s="1" t="n">
         <v>0.038979</v>
       </c>
+      <c r="D100" s="1"/>
       <c r="E100" s="5" t="n">
         <f aca="false">E99*(1+C100)</f>
         <v>4.81979054783453</v>
@@ -13317,6 +13416,7 @@
       <c r="C101" s="1" t="n">
         <v>0.037559</v>
       </c>
+      <c r="D101" s="1"/>
       <c r="E101" s="5" t="n">
         <f aca="false">E100*(1+C101)</f>
         <v>5.00081706102065</v>
@@ -13336,6 +13436,7 @@
       <c r="C102" s="1" t="n">
         <v>-0.023159</v>
       </c>
+      <c r="D102" s="1"/>
       <c r="E102" s="5" t="n">
         <f aca="false">E101*(1+C102)</f>
         <v>4.88500313870447</v>
@@ -13355,6 +13456,7 @@
       <c r="C103" s="1" t="n">
         <v>0.054431</v>
       </c>
+      <c r="D103" s="1"/>
       <c r="E103" s="5" t="n">
         <f aca="false">E102*(1+C103)</f>
         <v>5.15089874454729</v>
@@ -13374,6 +13476,7 @@
       <c r="C104" s="1" t="n">
         <v>-0.03022</v>
       </c>
+      <c r="D104" s="1"/>
       <c r="E104" s="5" t="n">
         <f aca="false">E103*(1+C104)</f>
         <v>4.99523858448707</v>
@@ -13393,6 +13496,7 @@
       <c r="C105" s="1" t="n">
         <v>-0.005004</v>
       </c>
+      <c r="D105" s="1"/>
       <c r="E105" s="5" t="n">
         <f aca="false">E104*(1+C105)</f>
         <v>4.9702424106103</v>
@@ -13412,6 +13516,7 @@
       <c r="C106" s="1" t="n">
         <v>-0.028079</v>
       </c>
+      <c r="D106" s="1"/>
       <c r="E106" s="5" t="n">
         <f aca="false">E105*(1+C106)</f>
         <v>4.83068297396277</v>
@@ -13431,6 +13536,7 @@
       <c r="C107" s="1" t="n">
         <v>0.064238</v>
       </c>
+      <c r="D107" s="1"/>
       <c r="E107" s="5" t="n">
         <f aca="false">E106*(1+C107)</f>
         <v>5.14099638684419</v>
@@ -13450,6 +13556,7 @@
       <c r="C108" s="1" t="n">
         <v>0.020822</v>
       </c>
+      <c r="D108" s="1"/>
       <c r="E108" s="5" t="n">
         <f aca="false">E107*(1+C108)</f>
         <v>5.24804221361106</v>
@@ -13469,6 +13576,7 @@
       <c r="C109" s="1" t="n">
         <v>0.062579</v>
       </c>
+      <c r="D109" s="1"/>
       <c r="E109" s="5" t="n">
         <f aca="false">E108*(1+C109)</f>
         <v>5.57645944729663</v>
@@ -13488,6 +13596,7 @@
       <c r="C110" s="1" t="n">
         <v>-0.04963</v>
       </c>
+      <c r="D110" s="1"/>
       <c r="E110" s="5" t="n">
         <f aca="false">E109*(1+C110)</f>
         <v>5.2996997649273</v>
@@ -13507,6 +13616,7 @@
       <c r="C111" s="1" t="n">
         <v>-0.017458</v>
       </c>
+      <c r="D111" s="1"/>
       <c r="E111" s="5" t="n">
         <f aca="false">E110*(1+C111)</f>
         <v>5.2071776064312</v>
@@ -13526,6 +13636,7 @@
       <c r="C112" s="1" t="n">
         <v>0.098488</v>
       </c>
+      <c r="D112" s="1"/>
       <c r="E112" s="5" t="n">
         <f aca="false">E111*(1+C112)</f>
         <v>5.72002211453339</v>
@@ -13545,6 +13656,7 @@
       <c r="C113" s="1" t="n">
         <v>-0.031583</v>
       </c>
+      <c r="D113" s="1"/>
       <c r="E113" s="5" t="n">
         <f aca="false">E112*(1+C113)</f>
         <v>5.53936665609008</v>
@@ -13564,6 +13676,7 @@
       <c r="C114" s="1" t="n">
         <v>-0.022304</v>
       </c>
+      <c r="D114" s="1"/>
       <c r="E114" s="5" t="n">
         <f aca="false">E113*(1+C114)</f>
         <v>5.41581662219265</v>
@@ -13583,6 +13696,7 @@
       <c r="C115" s="1" t="n">
         <v>0.026219</v>
       </c>
+      <c r="D115" s="1"/>
       <c r="E115" s="5" t="n">
         <f aca="false">E114*(1+C115)</f>
         <v>5.55781391820992</v>
@@ -13602,6 +13716,7 @@
       <c r="C116" s="1" t="n">
         <v>-0.012795</v>
       </c>
+      <c r="D116" s="1"/>
       <c r="E116" s="5" t="n">
         <f aca="false">E115*(1+C116)</f>
         <v>5.48670168912642</v>
@@ -13621,6 +13736,7 @@
       <c r="C117" s="1" t="n">
         <v>0.062594</v>
       </c>
+      <c r="D117" s="1"/>
       <c r="E117" s="5" t="n">
         <f aca="false">E116*(1+C117)</f>
         <v>5.8301362946556</v>
@@ -13640,6 +13756,7 @@
       <c r="C118" s="1" t="n">
         <v>-0.052088</v>
       </c>
+      <c r="D118" s="1"/>
       <c r="E118" s="5" t="n">
         <f aca="false">E117*(1+C118)</f>
         <v>5.52645615533958</v>
@@ -13659,6 +13776,7 @@
       <c r="C119" s="1" t="n">
         <v>-0.00412</v>
       </c>
+      <c r="D119" s="1"/>
       <c r="E119" s="5" t="n">
         <f aca="false">E118*(1+C119)</f>
         <v>5.50368715597958</v>
@@ -13678,6 +13796,7 @@
       <c r="C120" s="1" t="n">
         <v>-0.078268</v>
       </c>
+      <c r="D120" s="1"/>
       <c r="E120" s="5" t="n">
         <f aca="false">E119*(1+C120)</f>
         <v>5.07292456965537</v>
@@ -13697,6 +13816,7 @@
       <c r="C121" s="1" t="n">
         <v>0.00572</v>
       </c>
+      <c r="D121" s="1"/>
       <c r="E121" s="5" t="n">
         <f aca="false">E120*(1+C121)</f>
         <v>5.1019416981938</v>
@@ -13716,6 +13836,7 @@
       <c r="C122" s="1" t="n">
         <v>0.032372</v>
       </c>
+      <c r="D122" s="1"/>
       <c r="E122" s="5" t="n">
         <f aca="false">E121*(1+C122)</f>
         <v>5.26710175484773</v>
@@ -13735,6 +13856,7 @@
       <c r="C123" s="1" t="n">
         <v>-0.090952</v>
       </c>
+      <c r="D123" s="1"/>
       <c r="E123" s="5" t="n">
         <f aca="false">E122*(1+C123)</f>
         <v>4.78804831604082</v>
@@ -13754,6 +13876,7 @@
       <c r="C124" s="1" t="n">
         <v>-0.063706</v>
       </c>
+      <c r="D124" s="1"/>
       <c r="E124" s="5" t="n">
         <f aca="false">E123*(1+C124)</f>
         <v>4.48302091001912</v>
@@ -13773,6 +13896,7 @@
       <c r="C125" s="1" t="n">
         <v>0.077824</v>
       </c>
+      <c r="D125" s="1"/>
       <c r="E125" s="5" t="n">
         <f aca="false">E124*(1+C125)</f>
         <v>4.83190752932045</v>
@@ -13792,6 +13916,7 @@
       <c r="C126" s="1" t="n">
         <v>0.006859</v>
       </c>
+      <c r="D126" s="1"/>
       <c r="E126" s="5" t="n">
         <f aca="false">E125*(1+C126)</f>
         <v>4.86504958306406</v>
@@ -13811,6 +13936,7 @@
       <c r="C127" s="1" t="n">
         <v>-0.024505</v>
       </c>
+      <c r="D127" s="1"/>
       <c r="E127" s="5" t="n">
         <f aca="false">E126*(1+C127)</f>
         <v>4.74583154303108</v>
@@ -13830,6 +13956,7 @@
       <c r="C128" s="1" t="n">
         <v>-0.009317</v>
       </c>
+      <c r="D128" s="1"/>
       <c r="E128" s="5" t="n">
         <f aca="false">E127*(1+C128)</f>
         <v>4.70161463054466</v>
@@ -13849,6 +13976,7 @@
       <c r="C129" s="1" t="n">
         <v>-0.063435</v>
       </c>
+      <c r="D129" s="1"/>
       <c r="E129" s="5" t="n">
         <f aca="false">E128*(1+C129)</f>
         <v>4.40336770645606</v>
@@ -13868,6 +13996,7 @@
       <c r="C130" s="1" t="n">
         <v>-0.080361</v>
       </c>
+      <c r="D130" s="1"/>
       <c r="E130" s="5" t="n">
         <f aca="false">E129*(1+C130)</f>
         <v>4.04950867419754</v>
@@ -13887,6 +14016,7 @@
       <c r="C131" s="1" t="n">
         <v>0.01954</v>
       </c>
+      <c r="D131" s="1"/>
       <c r="E131" s="5" t="n">
         <f aca="false">E130*(1+C131)</f>
         <v>4.12863607369136</v>
@@ -13906,6 +14036,7 @@
       <c r="C132" s="1" t="n">
         <v>0.078787</v>
       </c>
+      <c r="D132" s="1"/>
       <c r="E132" s="5" t="n">
         <f aca="false">E131*(1+C132)</f>
         <v>4.45391892402928</v>
@@ -13925,6 +14056,7 @@
       <c r="C133" s="1" t="n">
         <v>0.009051</v>
       </c>
+      <c r="D133" s="1"/>
       <c r="E133" s="5" t="n">
         <f aca="false">E132*(1+C133)</f>
         <v>4.49423134421067</v>
@@ -13944,6 +14076,7 @@
       <c r="C134" s="1" t="n">
         <v>-0.014324</v>
       </c>
+      <c r="D134" s="1"/>
       <c r="E134" s="5" t="n">
         <f aca="false">E133*(1+C134)</f>
         <v>4.4298559744362</v>
@@ -13963,6 +14096,7 @@
       <c r="C135" s="1" t="n">
         <v>-0.019481</v>
       </c>
+      <c r="D135" s="1"/>
       <c r="E135" s="5" t="n">
         <f aca="false">E134*(1+C135)</f>
         <v>4.3435579501982</v>
@@ -13982,6 +14116,7 @@
       <c r="C136" s="1" t="n">
         <v>0.037572</v>
       </c>
+      <c r="D136" s="1"/>
       <c r="E136" s="5" t="n">
         <f aca="false">E135*(1+C136)</f>
         <v>4.50675410950305</v>
@@ -14001,6 +14136,7 @@
       <c r="C137" s="1" t="n">
         <v>-0.061001</v>
       </c>
+      <c r="D137" s="1"/>
       <c r="E137" s="5" t="n">
         <f aca="false">E136*(1+C137)</f>
         <v>4.23183760206925</v>
@@ -14020,6 +14156,7 @@
       <c r="C138" s="1" t="n">
         <v>-0.0078</v>
       </c>
+      <c r="D138" s="1"/>
       <c r="E138" s="5" t="n">
         <f aca="false">E137*(1+C138)</f>
         <v>4.19882926877311</v>
@@ -14039,6 +14176,7 @@
       <c r="C139" s="1" t="n">
         <v>-0.071349</v>
       </c>
+      <c r="D139" s="1"/>
       <c r="E139" s="5" t="n">
         <f aca="false">E138*(1+C139)</f>
         <v>3.89924699927542</v>
@@ -14058,6 +14196,7 @@
       <c r="C140" s="1" t="n">
         <v>-0.073987</v>
       </c>
+      <c r="D140" s="1"/>
       <c r="E140" s="5" t="n">
         <f aca="false">E139*(1+C140)</f>
         <v>3.61075341154003</v>
@@ -14077,6 +14216,7 @@
       <c r="C141" s="1" t="n">
         <v>0.007061</v>
       </c>
+      <c r="D141" s="1"/>
       <c r="E141" s="5" t="n">
         <f aca="false">E140*(1+C141)</f>
         <v>3.63624894137891</v>
@@ -14096,6 +14236,7 @@
       <c r="C142" s="1" t="n">
         <v>-0.108965</v>
       </c>
+      <c r="D142" s="1"/>
       <c r="E142" s="5" t="n">
         <f aca="false">E141*(1+C142)</f>
         <v>3.24002507548156</v>
@@ -14115,6 +14256,7 @@
       <c r="C143" s="1" t="n">
         <v>0.088599</v>
       </c>
+      <c r="D143" s="1"/>
       <c r="E143" s="5" t="n">
         <f aca="false">E142*(1+C143)</f>
         <v>3.52708805714415</v>
@@ -14134,6 +14276,7 @@
       <c r="C144" s="1" t="n">
         <v>0.059019</v>
       </c>
+      <c r="D144" s="1"/>
       <c r="E144" s="5" t="n">
         <f aca="false">E143*(1+C144)</f>
         <v>3.73525326718874</v>
@@ -14153,6 +14296,7 @@
       <c r="C145" s="1" t="n">
         <v>-0.058834</v>
       </c>
+      <c r="D145" s="1"/>
       <c r="E145" s="5" t="n">
         <f aca="false">E144*(1+C145)</f>
         <v>3.51549337646696</v>
@@ -14172,6 +14316,7 @@
       <c r="C146" s="1" t="n">
         <v>-0.026579</v>
       </c>
+      <c r="D146" s="1"/>
       <c r="E146" s="5" t="n">
         <f aca="false">E145*(1+C146)</f>
         <v>3.42205507801384</v>
@@ -14191,6 +14336,7 @@
       <c r="C147" s="1" t="n">
         <v>-0.015246</v>
       </c>
+      <c r="D147" s="1"/>
       <c r="E147" s="5" t="n">
         <f aca="false">E146*(1+C147)</f>
         <v>3.36988242629445</v>
@@ -14210,6 +14356,7 @@
       <c r="C148" s="1" t="n">
         <v>0.010308</v>
       </c>
+      <c r="D148" s="1"/>
       <c r="E148" s="5" t="n">
         <f aca="false">E147*(1+C148)</f>
         <v>3.40461917434469</v>
@@ -14229,6 +14376,7 @@
       <c r="C149" s="1" t="n">
         <v>0.082774</v>
       </c>
+      <c r="D149" s="1"/>
       <c r="E149" s="5" t="n">
         <f aca="false">E148*(1+C149)</f>
         <v>3.6864331218819</v>
@@ -14248,6 +14396,7 @@
       <c r="C150" s="1" t="n">
         <v>0.053251</v>
       </c>
+      <c r="D150" s="1"/>
       <c r="E150" s="5" t="n">
         <f aca="false">E149*(1+C150)</f>
         <v>3.88273937205523</v>
@@ -14267,6 +14416,7 @@
       <c r="C151" s="1" t="n">
         <v>0.012816</v>
       </c>
+      <c r="D151" s="1"/>
       <c r="E151" s="5" t="n">
         <f aca="false">E150*(1+C151)</f>
         <v>3.93250055984749</v>
@@ -14286,6 +14436,7 @@
       <c r="C152" s="1" t="n">
         <v>0.017932</v>
       </c>
+      <c r="D152" s="1"/>
       <c r="E152" s="5" t="n">
         <f aca="false">E151*(1+C152)</f>
         <v>4.00301815988667</v>
@@ -14305,6 +14456,7 @@
       <c r="C153" s="1" t="n">
         <v>0.019597</v>
       </c>
+      <c r="D153" s="1"/>
       <c r="E153" s="5" t="n">
         <f aca="false">E152*(1+C153)</f>
         <v>4.08146530676597</v>
@@ -14324,6 +14476,7 @@
       <c r="C154" s="1" t="n">
         <v>-0.010737</v>
       </c>
+      <c r="D154" s="1"/>
       <c r="E154" s="5" t="n">
         <f aca="false">E153*(1+C154)</f>
         <v>4.03764261376723</v>
@@ -14343,6 +14496,7 @@
       <c r="C155" s="1" t="n">
         <v>0.05556</v>
       </c>
+      <c r="D155" s="1"/>
       <c r="E155" s="5" t="n">
         <f aca="false">E154*(1+C155)</f>
         <v>4.26197403738813</v>
@@ -14362,6 +14516,7 @@
       <c r="C156" s="1" t="n">
         <v>0.009259</v>
       </c>
+      <c r="D156" s="1"/>
       <c r="E156" s="5" t="n">
         <f aca="false">E155*(1+C156)</f>
         <v>4.30143565500031</v>
@@ -14381,6 +14536,7 @@
       <c r="C157" s="1" t="n">
         <v>0.05178</v>
       </c>
+      <c r="D157" s="1"/>
       <c r="E157" s="5" t="n">
         <f aca="false">E156*(1+C157)</f>
         <v>4.52416399321623</v>
@@ -14400,6 +14556,7 @@
       <c r="C158" s="1" t="n">
         <v>0.019078</v>
       </c>
+      <c r="D158" s="1"/>
       <c r="E158" s="5" t="n">
         <f aca="false">E157*(1+C158)</f>
         <v>4.61047599387881</v>
@@ -14419,6 +14576,7 @@
       <c r="C159" s="1" t="n">
         <v>0.014403</v>
       </c>
+      <c r="D159" s="1"/>
       <c r="E159" s="5" t="n">
         <f aca="false">E158*(1+C159)</f>
         <v>4.67688067961864</v>
@@ -14438,6 +14596,7 @@
       <c r="C160" s="1" t="n">
         <v>-0.014982</v>
       </c>
+      <c r="D160" s="1"/>
       <c r="E160" s="5" t="n">
         <f aca="false">E159*(1+C160)</f>
         <v>4.60681165327659</v>
@@ -14457,6 +14616,7 @@
       <c r="C161" s="1" t="n">
         <v>-0.015584</v>
       </c>
+      <c r="D161" s="1"/>
       <c r="E161" s="5" t="n">
         <f aca="false">E160*(1+C161)</f>
         <v>4.53501910047193</v>
@@ -14476,6 +14636,7 @@
       <c r="C162" s="1" t="n">
         <v>0.013629</v>
       </c>
+      <c r="D162" s="1"/>
       <c r="E162" s="5" t="n">
         <f aca="false">E161*(1+C162)</f>
         <v>4.59682687579226</v>
@@ -14495,6 +14656,7 @@
       <c r="C163" s="1" t="n">
         <v>0.019489</v>
       </c>
+      <c r="D163" s="1"/>
       <c r="E163" s="5" t="n">
         <f aca="false">E162*(1+C163)</f>
         <v>4.68641443477458</v>
@@ -14514,6 +14676,7 @@
       <c r="C164" s="1" t="n">
         <v>-0.032954</v>
       </c>
+      <c r="D164" s="1"/>
       <c r="E164" s="5" t="n">
         <f aca="false">E163*(1+C164)</f>
         <v>4.53197833349102</v>
@@ -14533,6 +14696,7 @@
       <c r="C165" s="1" t="n">
         <v>0.003807</v>
       </c>
+      <c r="D165" s="1"/>
       <c r="E165" s="5" t="n">
         <f aca="false">E164*(1+C165)</f>
         <v>4.54923157500662</v>
@@ -14552,6 +14716,7 @@
       <c r="C166" s="1" t="n">
         <v>0.010817</v>
       </c>
+      <c r="D166" s="1"/>
       <c r="E166" s="5" t="n">
         <f aca="false">E165*(1+C166)</f>
         <v>4.59844061295346</v>
@@ -14571,6 +14736,7 @@
       <c r="C167" s="1" t="n">
         <v>0.014973</v>
       </c>
+      <c r="D167" s="1"/>
       <c r="E167" s="5" t="n">
         <f aca="false">E166*(1+C167)</f>
         <v>4.66729306425122</v>
@@ -14590,6 +14756,7 @@
       <c r="C168" s="1" t="n">
         <v>0.040559</v>
       </c>
+      <c r="D168" s="1"/>
       <c r="E168" s="5" t="n">
         <f aca="false">E167*(1+C168)</f>
         <v>4.85659380364418</v>
@@ -14609,6 +14776,7 @@
       <c r="C169" s="1" t="n">
         <v>0.033734</v>
       </c>
+      <c r="D169" s="1"/>
       <c r="E169" s="5" t="n">
         <f aca="false">E168*(1+C169)</f>
         <v>5.02042613901631</v>
@@ -14628,6 +14796,7 @@
       <c r="C170" s="1" t="n">
         <v>-0.023824</v>
       </c>
+      <c r="D170" s="1"/>
       <c r="E170" s="5" t="n">
         <f aca="false">E169*(1+C170)</f>
         <v>4.90081950668039</v>
@@ -14647,6 +14816,7 @@
       <c r="C171" s="1" t="n">
         <v>0.021152</v>
       </c>
+      <c r="D171" s="1"/>
       <c r="E171" s="5" t="n">
         <f aca="false">E170*(1+C171)</f>
         <v>5.00448164088569</v>
@@ -14666,6 +14836,7 @@
       <c r="C172" s="1" t="n">
         <v>-0.01724</v>
       </c>
+      <c r="D172" s="1"/>
       <c r="E172" s="5" t="n">
         <f aca="false">E171*(1+C172)</f>
         <v>4.91820437739682</v>
@@ -14685,6 +14856,7 @@
       <c r="C173" s="1" t="n">
         <v>-0.018926</v>
       </c>
+      <c r="D173" s="1"/>
       <c r="E173" s="5" t="n">
         <f aca="false">E172*(1+C173)</f>
         <v>4.82512244135021</v>
@@ -14704,6 +14876,7 @@
       <c r="C174" s="1" t="n">
         <v>0.031994</v>
       </c>
+      <c r="D174" s="1"/>
       <c r="E174" s="5" t="n">
         <f aca="false">E173*(1+C174)</f>
         <v>4.97949740873877</v>
@@ -14723,6 +14896,7 @@
       <c r="C175" s="1" t="n">
         <v>0.001717</v>
       </c>
+      <c r="D175" s="1"/>
       <c r="E175" s="5" t="n">
         <f aca="false">E174*(1+C175)</f>
         <v>4.98804720578957</v>
@@ -14742,6 +14916,7 @@
       <c r="C176" s="1" t="n">
         <v>0.037364</v>
       </c>
+      <c r="D176" s="1"/>
       <c r="E176" s="5" t="n">
         <f aca="false">E175*(1+C176)</f>
         <v>5.17442060158669</v>
@@ -14761,6 +14936,7 @@
       <c r="C177" s="1" t="n">
         <v>-0.009159</v>
       </c>
+      <c r="D177" s="1"/>
       <c r="E177" s="5" t="n">
         <f aca="false">E176*(1+C177)</f>
         <v>5.12702808329676</v>
@@ -14780,6 +14956,7 @@
       <c r="C178" s="1" t="n">
         <v>0.008067</v>
       </c>
+      <c r="D178" s="1"/>
       <c r="E178" s="5" t="n">
         <f aca="false">E177*(1+C178)</f>
         <v>5.16838781884472</v>
@@ -14799,6 +14976,7 @@
       <c r="C179" s="1" t="n">
         <v>-0.015672</v>
       </c>
+      <c r="D179" s="1"/>
       <c r="E179" s="5" t="n">
         <f aca="false">E178*(1+C179)</f>
         <v>5.08738884494778</v>
@@ -14818,6 +14996,7 @@
       <c r="C180" s="1" t="n">
         <v>0.038289</v>
       </c>
+      <c r="D180" s="1"/>
       <c r="E180" s="5" t="n">
         <f aca="false">E179*(1+C180)</f>
         <v>5.28217987643199</v>
@@ -14837,6 +15016,7 @@
       <c r="C181" s="1" t="n">
         <v>-6E-005</v>
       </c>
+      <c r="D181" s="1"/>
       <c r="E181" s="5" t="n">
         <f aca="false">E180*(1+C181)</f>
         <v>5.2818629456394</v>
@@ -14856,6 +15036,7 @@
       <c r="C182" s="1" t="n">
         <v>0.026442</v>
       </c>
+      <c r="D182" s="1"/>
       <c r="E182" s="5" t="n">
         <f aca="false">E181*(1+C182)</f>
         <v>5.421525965648</v>
@@ -14875,6 +15056,7 @@
       <c r="C183" s="1" t="n">
         <v>0.002425</v>
       </c>
+      <c r="D183" s="1"/>
       <c r="E183" s="5" t="n">
         <f aca="false">E182*(1+C183)</f>
         <v>5.43467316611469</v>
@@ -14894,6 +15076,7 @@
       <c r="C184" s="1" t="n">
         <v>0.012909</v>
       </c>
+      <c r="D184" s="1"/>
       <c r="E184" s="5" t="n">
         <f aca="false">E183*(1+C184)</f>
         <v>5.50482936201607</v>
@@ -14913,6 +15096,7 @@
       <c r="C185" s="1" t="n">
         <v>0.012064</v>
       </c>
+      <c r="D185" s="1"/>
       <c r="E185" s="5" t="n">
         <f aca="false">E184*(1+C185)</f>
         <v>5.57123962343943</v>
@@ -14932,6 +15116,7 @@
       <c r="C186" s="1" t="n">
         <v>-0.028319</v>
       </c>
+      <c r="D186" s="1"/>
       <c r="E186" s="5" t="n">
         <f aca="false">E185*(1+C186)</f>
         <v>5.41346768854325</v>
@@ -14951,6 +15136,7 @@
       <c r="C187" s="1" t="n">
         <v>0.001587</v>
       </c>
+      <c r="D187" s="1"/>
       <c r="E187" s="5" t="n">
         <f aca="false">E186*(1+C187)</f>
         <v>5.42205886176497</v>
@@ -14970,6 +15156,7 @@
       <c r="C188" s="1" t="n">
         <v>0.005571</v>
       </c>
+      <c r="D188" s="1"/>
       <c r="E188" s="5" t="n">
         <f aca="false">E187*(1+C188)</f>
         <v>5.45226515168386</v>
@@ -14989,6 +15176,7 @@
       <c r="C189" s="1" t="n">
         <v>0.02415</v>
       </c>
+      <c r="D189" s="1"/>
       <c r="E189" s="5" t="n">
         <f aca="false">E188*(1+C189)</f>
         <v>5.58393735509702</v>
@@ -15008,6 +15196,7 @@
       <c r="C190" s="1" t="n">
         <v>0.026487</v>
       </c>
+      <c r="D190" s="1"/>
       <c r="E190" s="5" t="n">
         <f aca="false">E189*(1+C190)</f>
         <v>5.73183910382148</v>
@@ -15027,6 +15216,7 @@
       <c r="C191" s="1" t="n">
         <v>0.032527</v>
       </c>
+      <c r="D191" s="1"/>
       <c r="E191" s="5" t="n">
         <f aca="false">E190*(1+C191)</f>
         <v>5.91827863435148</v>
@@ -15046,6 +15236,7 @@
       <c r="C192" s="1" t="n">
         <v>0.018385</v>
       </c>
+      <c r="D192" s="1"/>
       <c r="E192" s="5" t="n">
         <f aca="false">E191*(1+C192)</f>
         <v>6.02708618704403</v>
@@ -15065,6 +15256,7 @@
       <c r="C193" s="1" t="n">
         <v>0.013768</v>
       </c>
+      <c r="D193" s="1"/>
       <c r="E193" s="5" t="n">
         <f aca="false">E192*(1+C193)</f>
         <v>6.11006710966726</v>
@@ -15084,6 +15276,7 @@
       <c r="C194" s="1" t="n">
         <v>0.015313</v>
       </c>
+      <c r="D194" s="1"/>
       <c r="E194" s="5" t="n">
         <f aca="false">E193*(1+C194)</f>
         <v>6.20363056731759</v>
@@ -15103,6 +15296,7 @@
       <c r="C195" s="1" t="n">
         <v>-0.019288</v>
       </c>
+      <c r="D195" s="1"/>
       <c r="E195" s="5" t="n">
         <f aca="false">E194*(1+C195)</f>
         <v>6.08397494093517</v>
@@ -15122,6 +15316,7 @@
       <c r="C196" s="1" t="n">
         <v>0.010894</v>
       </c>
+      <c r="D196" s="1"/>
       <c r="E196" s="5" t="n">
         <f aca="false">E195*(1+C196)</f>
         <v>6.15025376394172</v>
@@ -15141,6 +15336,7 @@
       <c r="C197" s="1" t="n">
         <v>0.043991</v>
       </c>
+      <c r="D197" s="1"/>
       <c r="E197" s="5" t="n">
         <f aca="false">E196*(1+C197)</f>
         <v>6.42080957727128</v>
@@ -15160,6 +15356,7 @@
       <c r="C198" s="1" t="n">
         <v>0.034459</v>
       </c>
+      <c r="D198" s="1"/>
       <c r="E198" s="5" t="n">
         <f aca="false">E197*(1+C198)</f>
         <v>6.64206425449447</v>
@@ -15179,6 +15376,7 @@
       <c r="C199" s="1" t="n">
         <v>-0.01662</v>
       </c>
+      <c r="D199" s="1"/>
       <c r="E199" s="5" t="n">
         <f aca="false">E198*(1+C199)</f>
         <v>6.53167314658477</v>
@@ -15198,6 +15396,7 @@
       <c r="C200" s="1" t="n">
         <v>-0.031197</v>
       </c>
+      <c r="D200" s="1"/>
       <c r="E200" s="5" t="n">
         <f aca="false">E199*(1+C200)</f>
         <v>6.32790453943076</v>
@@ -15217,6 +15416,7 @@
       <c r="C201" s="1" t="n">
         <v>0.015094</v>
       </c>
+      <c r="D201" s="1"/>
       <c r="E201" s="5" t="n">
         <f aca="false">E200*(1+C201)</f>
         <v>6.42341793054893</v>
@@ -15236,6 +15436,7 @@
       <c r="C202" s="1" t="n">
         <v>0.037468</v>
       </c>
+      <c r="D202" s="1"/>
       <c r="E202" s="5" t="n">
         <f aca="false">E201*(1+C202)</f>
         <v>6.66409055357074</v>
@@ -15255,6 +15456,7 @@
       <c r="C203" s="1" t="n">
         <v>0.01736</v>
       </c>
+      <c r="D203" s="1"/>
       <c r="E203" s="5" t="n">
         <f aca="false">E202*(1+C203)</f>
         <v>6.77977916558073</v>
@@ -15274,6 +15476,7 @@
       <c r="C204" s="1" t="n">
         <v>-0.041382</v>
       </c>
+      <c r="D204" s="1"/>
       <c r="E204" s="5" t="n">
         <f aca="false">E203*(1+C204)</f>
         <v>6.49921834415067</v>
@@ -15293,6 +15496,7 @@
       <c r="C205" s="1" t="n">
         <v>-0.006116</v>
       </c>
+      <c r="D205" s="1"/>
       <c r="E205" s="5" t="n">
         <f aca="false">E204*(1+C205)</f>
         <v>6.45946912475784</v>
@@ -15312,6 +15516,7 @@
       <c r="C206" s="1" t="n">
         <v>-0.061166</v>
       </c>
+      <c r="D206" s="1"/>
       <c r="E206" s="5" t="n">
         <f aca="false">E205*(1+C206)</f>
         <v>6.0643692362729</v>
@@ -15331,6 +15536,7 @@
       <c r="C207" s="1" t="n">
         <v>-0.031419</v>
       </c>
+      <c r="D207" s="1"/>
       <c r="E207" s="5" t="n">
         <f aca="false">E206*(1+C207)</f>
         <v>5.87383281923844</v>
@@ -15350,6 +15556,7 @@
       <c r="C208" s="1" t="n">
         <v>-0.0034</v>
       </c>
+      <c r="D208" s="1"/>
       <c r="E208" s="5" t="n">
         <f aca="false">E207*(1+C208)</f>
         <v>5.85386178765303</v>
@@ -15369,6 +15576,7 @@
       <c r="C209" s="1" t="n">
         <v>0.048629</v>
       </c>
+      <c r="D209" s="1"/>
       <c r="E209" s="5" t="n">
         <f aca="false">E208*(1+C209)</f>
         <v>6.13852923252481</v>
@@ -15388,6 +15596,7 @@
       <c r="C210" s="1" t="n">
         <v>0.012986</v>
       </c>
+      <c r="D210" s="1"/>
       <c r="E210" s="5" t="n">
         <f aca="false">E209*(1+C210)</f>
         <v>6.21824417313838</v>
@@ -15407,6 +15616,7 @@
       <c r="C211" s="1" t="n">
         <v>-0.082842</v>
       </c>
+      <c r="D211" s="1"/>
       <c r="E211" s="5" t="n">
         <f aca="false">E210*(1+C211)</f>
         <v>5.70311238934725</v>
@@ -15426,6 +15636,7 @@
       <c r="C212" s="1" t="n">
         <v>-0.007306</v>
       </c>
+      <c r="D212" s="1"/>
       <c r="E212" s="5" t="n">
         <f aca="false">E211*(1+C212)</f>
         <v>5.66144545023068</v>
@@ -15445,6 +15656,7 @@
       <c r="C213" s="1" t="n">
         <v>0.014955</v>
       </c>
+      <c r="D213" s="1"/>
       <c r="E213" s="5" t="n">
         <f aca="false">E212*(1+C213)</f>
         <v>5.74611236693888</v>
@@ -15464,6 +15676,7 @@
       <c r="C214" s="1" t="n">
         <v>-0.085467</v>
       </c>
+      <c r="D214" s="1"/>
       <c r="E214" s="5" t="n">
         <f aca="false">E213*(1+C214)</f>
         <v>5.25500938127371</v>
@@ -15483,6 +15696,7 @@
       <c r="C215" s="1" t="n">
         <v>-0.16698</v>
       </c>
+      <c r="D215" s="1"/>
       <c r="E215" s="5" t="n">
         <f aca="false">E214*(1+C215)</f>
         <v>4.37752791478863</v>
@@ -15502,6 +15716,7 @@
       <c r="C216" s="1" t="n">
         <v>-0.073512</v>
       </c>
+      <c r="D216" s="1"/>
       <c r="E216" s="5" t="n">
         <f aca="false">E215*(1+C216)</f>
         <v>4.05572708271669</v>
@@ -15521,6 +15736,7 @@
       <c r="C217" s="1" t="n">
         <v>0.011996</v>
       </c>
+      <c r="D217" s="1"/>
       <c r="E217" s="5" t="n">
         <f aca="false">E216*(1+C217)</f>
         <v>4.10437958480096</v>
@@ -15540,6 +15756,7 @@
       <c r="C218" s="1" t="n">
         <v>-0.082615</v>
       </c>
+      <c r="D218" s="1"/>
       <c r="E218" s="5" t="n">
         <f aca="false">E217*(1+C218)</f>
         <v>3.76529626540262</v>
@@ -15559,6 +15776,7 @@
       <c r="C219" s="1" t="n">
         <v>-0.103588</v>
       </c>
+      <c r="D219" s="1"/>
       <c r="E219" s="5" t="n">
         <f aca="false">E218*(1+C219)</f>
         <v>3.3752567558621</v>
@@ -15578,6 +15796,7 @@
       <c r="C220" s="1" t="n">
         <v>0.087634</v>
       </c>
+      <c r="D220" s="1"/>
       <c r="E220" s="5" t="n">
         <f aca="false">E219*(1+C220)</f>
         <v>3.67104400640532</v>
@@ -15597,6 +15816,7 @@
       <c r="C221" s="1" t="n">
         <v>0.09423</v>
       </c>
+      <c r="D221" s="1"/>
       <c r="E221" s="5" t="n">
         <f aca="false">E220*(1+C221)</f>
         <v>4.01696648312889</v>
@@ -15616,6 +15836,7 @@
       <c r="C222" s="1" t="n">
         <v>0.05464</v>
       </c>
+      <c r="D222" s="1"/>
       <c r="E222" s="5" t="n">
         <f aca="false">E221*(1+C222)</f>
         <v>4.23645353176705</v>
@@ -15635,6 +15856,7 @@
       <c r="C223" s="1" t="n">
         <v>0.002476</v>
       </c>
+      <c r="D223" s="1"/>
       <c r="E223" s="5" t="n">
         <f aca="false">E222*(1+C223)</f>
         <v>4.24694299071171</v>
@@ -15654,6 +15876,7 @@
       <c r="C224" s="1" t="n">
         <v>0.074482</v>
       </c>
+      <c r="D224" s="1"/>
       <c r="E224" s="5" t="n">
         <f aca="false">E223*(1+C224)</f>
         <v>4.5632637985459</v>
@@ -15673,6 +15896,7 @@
       <c r="C225" s="1" t="n">
         <v>0.034751</v>
       </c>
+      <c r="D225" s="1"/>
       <c r="E225" s="5" t="n">
         <f aca="false">E224*(1+C225)</f>
         <v>4.72184177880916</v>
@@ -15692,6 +15916,7 @@
       <c r="C226" s="1" t="n">
         <v>0.036534</v>
       </c>
+      <c r="D226" s="1"/>
       <c r="E226" s="5" t="n">
         <f aca="false">E225*(1+C226)</f>
         <v>4.89434954635618</v>
@@ -15711,6 +15936,7 @@
       <c r="C227" s="1" t="n">
         <v>-0.018259</v>
       </c>
+      <c r="D227" s="1"/>
       <c r="E227" s="5" t="n">
         <f aca="false">E226*(1+C227)</f>
         <v>4.80498361798926</v>
@@ -15730,6 +15956,7 @@
       <c r="C228" s="1" t="n">
         <v>0.060257</v>
       </c>
+      <c r="D228" s="1"/>
       <c r="E228" s="5" t="n">
         <f aca="false">E227*(1+C228)</f>
         <v>5.09451751585844</v>
@@ -15749,6 +15976,7 @@
       <c r="C229" s="1" t="n">
         <v>0.018983</v>
       </c>
+      <c r="D229" s="1"/>
       <c r="E229" s="5" t="n">
         <f aca="false">E228*(1+C229)</f>
         <v>5.19122674186198</v>
@@ -15768,6 +15996,7 @@
       <c r="C230" s="1" t="n">
         <v>-0.035751</v>
       </c>
+      <c r="D230" s="1"/>
       <c r="E230" s="5" t="n">
         <f aca="false">E229*(1+C230)</f>
         <v>5.00563519461367</v>
@@ -15787,6 +16016,7 @@
       <c r="C231" s="1" t="n">
         <v>0.030424</v>
       </c>
+      <c r="D231" s="1"/>
       <c r="E231" s="5" t="n">
         <f aca="false">E230*(1+C231)</f>
         <v>5.1579266397746</v>
@@ -15806,6 +16036,7 @@
       <c r="C232" s="1" t="n">
         <v>0.061014</v>
       </c>
+      <c r="D232" s="1"/>
       <c r="E232" s="5" t="n">
         <f aca="false">E231*(1+C232)</f>
         <v>5.47263237577381</v>
@@ -15825,6 +16056,7 @@
       <c r="C233" s="1" t="n">
         <v>0.015977</v>
       </c>
+      <c r="D233" s="1"/>
       <c r="E233" s="5" t="n">
         <f aca="false">E232*(1+C233)</f>
         <v>5.56006862324154</v>
@@ -15844,6 +16076,7 @@
       <c r="C234" s="1" t="n">
         <v>-0.080111</v>
       </c>
+      <c r="D234" s="1"/>
       <c r="E234" s="5" t="n">
         <f aca="false">E233*(1+C234)</f>
         <v>5.11464596576504</v>
@@ -15863,6 +16096,7 @@
       <c r="C235" s="1" t="n">
         <v>-0.053525</v>
       </c>
+      <c r="D235" s="1"/>
       <c r="E235" s="5" t="n">
         <f aca="false">E234*(1+C235)</f>
         <v>4.84088454044747</v>
@@ -15882,6 +16116,7 @@
       <c r="C236" s="1" t="n">
         <v>0.070451</v>
       </c>
+      <c r="D236" s="1"/>
       <c r="E236" s="5" t="n">
         <f aca="false">E235*(1+C236)</f>
         <v>5.18192969720653</v>
@@ -15901,6 +16136,7 @@
       <c r="C237" s="1" t="n">
         <v>-0.045434</v>
       </c>
+      <c r="D237" s="1"/>
       <c r="E237" s="5" t="n">
         <f aca="false">E236*(1+C237)</f>
         <v>4.94649390334365</v>
@@ -15920,6 +16156,7 @@
       <c r="C238" s="1" t="n">
         <v>0.090383</v>
       </c>
+      <c r="D238" s="1"/>
       <c r="E238" s="5" t="n">
         <f aca="false">E237*(1+C238)</f>
         <v>5.39357286180956</v>
@@ -15939,6 +16176,7 @@
       <c r="C239" s="1" t="n">
         <v>0.038726</v>
       </c>
+      <c r="D239" s="1"/>
       <c r="E239" s="5" t="n">
         <f aca="false">E238*(1+C239)</f>
         <v>5.602444364456</v>
@@ -15958,6 +16196,7 @@
       <c r="C240" s="1" t="n">
         <v>-5.1E-005</v>
       </c>
+      <c r="D240" s="1"/>
       <c r="E240" s="5" t="n">
         <f aca="false">E239*(1+C240)</f>
         <v>5.60215863979341</v>
@@ -15977,6 +16216,7 @@
       <c r="C241" s="1" t="n">
         <v>0.067055</v>
       </c>
+      <c r="D241" s="1"/>
       <c r="E241" s="5" t="n">
         <f aca="false">E240*(1+C241)</f>
         <v>5.97781138738476</v>
@@ -15996,6 +16236,7 @@
       <c r="C242" s="1" t="n">
         <v>0.023349</v>
       </c>
+      <c r="D242" s="1"/>
       <c r="E242" s="5" t="n">
         <f aca="false">E241*(1+C242)</f>
         <v>6.1173873054688</v>
@@ -16015,6 +16256,7 @@
       <c r="C243" s="1" t="n">
         <v>0.032508</v>
       </c>
+      <c r="D243" s="1"/>
       <c r="E243" s="5" t="n">
         <f aca="false">E242*(1+C243)</f>
         <v>6.31625133199498</v>
@@ -16034,6 +16276,7 @@
       <c r="C244" s="1" t="n">
         <v>0.000625</v>
       </c>
+      <c r="D244" s="1"/>
       <c r="E244" s="5" t="n">
         <f aca="false">E243*(1+C244)</f>
         <v>6.32019898907748</v>
@@ -16053,6 +16296,7 @@
       <c r="C245" s="1" t="n">
         <v>0.029441</v>
       </c>
+      <c r="D245" s="1"/>
       <c r="E245" s="5" t="n">
         <f aca="false">E244*(1+C245)</f>
         <v>6.50627196751491</v>
@@ -16072,6 +16316,7 @@
       <c r="C246" s="1" t="n">
         <v>-0.011313</v>
       </c>
+      <c r="D246" s="1"/>
       <c r="E246" s="5" t="n">
         <f aca="false">E245*(1+C246)</f>
         <v>6.43266651274642</v>
@@ -16091,6 +16336,7 @@
       <c r="C247" s="1" t="n">
         <v>-0.016545</v>
       </c>
+      <c r="D247" s="1"/>
       <c r="E247" s="5" t="n">
         <f aca="false">E246*(1+C247)</f>
         <v>6.32623804529303</v>
@@ -16110,6 +16356,7 @@
       <c r="C248" s="1" t="n">
         <v>-0.019828</v>
       </c>
+      <c r="D248" s="1"/>
       <c r="E248" s="5" t="n">
         <f aca="false">E247*(1+C248)</f>
         <v>6.20080139733096</v>
@@ -16129,6 +16376,7 @@
       <c r="C249" s="1" t="n">
         <v>-0.054323</v>
       </c>
+      <c r="D249" s="1"/>
       <c r="E249" s="5" t="n">
         <f aca="false">E248*(1+C249)</f>
         <v>5.86395526302375</v>
@@ -16148,6 +16396,7 @@
       <c r="C250" s="1" t="n">
         <v>-0.070238</v>
       </c>
+      <c r="D250" s="1"/>
       <c r="E250" s="5" t="n">
         <f aca="false">E249*(1+C250)</f>
         <v>5.45208277325949</v>
@@ -16167,6 +16416,7 @@
       <c r="C251" s="1" t="n">
         <v>0.109014</v>
       </c>
+      <c r="D251" s="1"/>
       <c r="E251" s="5" t="n">
         <f aca="false">E250*(1+C251)</f>
         <v>6.04643612470359</v>
@@ -16186,6 +16436,7 @@
       <c r="C252" s="1" t="n">
         <v>-0.002727</v>
       </c>
+      <c r="D252" s="1"/>
       <c r="E252" s="5" t="n">
         <f aca="false">E251*(1+C252)</f>
         <v>6.02994749339153</v>
@@ -16205,6 +16456,7 @@
       <c r="C253" s="1" t="n">
         <v>0.009427</v>
       </c>
+      <c r="D253" s="1"/>
       <c r="E253" s="5" t="n">
         <f aca="false">E252*(1+C253)</f>
         <v>6.08679180841173</v>
@@ -16224,6 +16476,7 @@
       <c r="C254" s="1" t="n">
         <v>0.045205</v>
       </c>
+      <c r="D254" s="1"/>
       <c r="E254" s="5" t="n">
         <f aca="false">E253*(1+C254)</f>
         <v>6.36194523211098</v>
@@ -16243,6 +16496,7 @@
       <c r="C255" s="1" t="n">
         <v>0.043341</v>
       </c>
+      <c r="D255" s="1"/>
       <c r="E255" s="5" t="n">
         <f aca="false">E254*(1+C255)</f>
         <v>6.6376783004159</v>
@@ -16262,6 +16516,7 @@
       <c r="C256" s="1" t="n">
         <v>0.032866</v>
       </c>
+      <c r="D256" s="1"/>
       <c r="E256" s="5" t="n">
         <f aca="false">E255*(1+C256)</f>
         <v>6.85583223543737</v>
@@ -16281,6 +16536,7 @@
       <c r="C257" s="1" t="n">
         <v>-0.006034</v>
       </c>
+      <c r="D257" s="1"/>
       <c r="E257" s="5" t="n">
         <f aca="false">E256*(1+C257)</f>
         <v>6.81446414372874</v>
@@ -16300,6 +16556,7 @@
       <c r="C258" s="1" t="n">
         <v>-0.05979</v>
       </c>
+      <c r="D258" s="1"/>
       <c r="E258" s="5" t="n">
         <f aca="false">E257*(1+C258)</f>
         <v>6.4070273325752</v>
@@ -16319,6 +16576,7 @@
       <c r="C259" s="1" t="n">
         <v>0.041465</v>
       </c>
+      <c r="D259" s="1"/>
       <c r="E259" s="5" t="n">
         <f aca="false">E258*(1+C259)</f>
         <v>6.67269472092043</v>
@@ -16338,6 +16596,7 @@
       <c r="C260" s="1" t="n">
         <v>0.014363</v>
       </c>
+      <c r="D260" s="1"/>
       <c r="E260" s="5" t="n">
         <f aca="false">E259*(1+C260)</f>
         <v>6.76853463519701</v>
@@ -16357,6 +16616,7 @@
       <c r="C261" s="1" t="n">
         <v>0.022744</v>
       </c>
+      <c r="D261" s="1"/>
       <c r="E261" s="5" t="n">
         <f aca="false">E260*(1+C261)</f>
         <v>6.92247818693993</v>
@@ -16376,6 +16636,7 @@
       <c r="C262" s="1" t="n">
         <v>0.02512</v>
       </c>
+      <c r="D262" s="1"/>
       <c r="E262" s="5" t="n">
         <f aca="false">E261*(1+C262)</f>
         <v>7.09637083899587</v>
@@ -16395,6 +16656,7 @@
       <c r="C263" s="1" t="n">
         <v>-0.017837</v>
       </c>
+      <c r="D263" s="1"/>
       <c r="E263" s="5" t="n">
         <f aca="false">E262*(1+C263)</f>
         <v>6.9697928723407</v>
@@ -16414,6 +16676,7 @@
       <c r="C264" s="1" t="n">
         <v>0.005326</v>
       </c>
+      <c r="D264" s="1"/>
       <c r="E264" s="5" t="n">
         <f aca="false">E263*(1+C264)</f>
         <v>7.00691398917878</v>
@@ -16433,6 +16696,7 @@
       <c r="C265" s="1" t="n">
         <v>0.008508</v>
       </c>
+      <c r="D265" s="1"/>
       <c r="E265" s="5" t="n">
         <f aca="false">E264*(1+C265)</f>
         <v>7.06652881339872</v>
@@ -16452,6 +16716,7 @@
       <c r="C266" s="1" t="n">
         <v>0.052361</v>
       </c>
+      <c r="D266" s="1"/>
       <c r="E266" s="5" t="n">
         <f aca="false">E265*(1+C266)</f>
         <v>7.43653932859709</v>
@@ -16471,6 +16736,7 @@
       <c r="C267" s="1" t="n">
         <v>0.013013</v>
       </c>
+      <c r="D267" s="1"/>
       <c r="E267" s="5" t="n">
         <f aca="false">E266*(1+C267)</f>
         <v>7.53331101488012</v>
@@ -16490,6 +16756,7 @@
       <c r="C268" s="1" t="n">
         <v>0.037584</v>
       </c>
+      <c r="D268" s="1"/>
       <c r="E268" s="5" t="n">
         <f aca="false">E267*(1+C268)</f>
         <v>7.81644297606337</v>
@@ -16509,6 +16776,7 @@
       <c r="C269" s="1" t="n">
         <v>0.019622</v>
       </c>
+      <c r="D269" s="1"/>
       <c r="E269" s="5" t="n">
         <f aca="false">E268*(1+C269)</f>
         <v>7.96981722013969</v>
@@ -16528,6 +16796,7 @@
       <c r="C270" s="1" t="n">
         <v>0.02312</v>
       </c>
+      <c r="D270" s="1"/>
       <c r="E270" s="5" t="n">
         <f aca="false">E269*(1+C270)</f>
         <v>8.15407939426932</v>
@@ -16547,6 +16816,7 @@
       <c r="C271" s="1" t="n">
         <v>-0.013601</v>
       </c>
+      <c r="D271" s="1"/>
       <c r="E271" s="5" t="n">
         <f aca="false">E270*(1+C271)</f>
         <v>8.04317576042786</v>
@@ -16566,6 +16836,7 @@
       <c r="C272" s="1" t="n">
         <v>0.050672</v>
       </c>
+      <c r="D272" s="1"/>
       <c r="E272" s="5" t="n">
         <f aca="false">E271*(1+C272)</f>
         <v>8.45073956256027</v>
@@ -16585,6 +16856,7 @@
       <c r="C273" s="1" t="n">
         <v>-0.029207</v>
       </c>
+      <c r="D273" s="1"/>
       <c r="E273" s="5" t="n">
         <f aca="false">E272*(1+C273)</f>
         <v>8.20391881215657</v>
@@ -16604,6 +16876,7 @@
       <c r="C274" s="1" t="n">
         <v>0.03166</v>
       </c>
+      <c r="D274" s="1"/>
       <c r="E274" s="5" t="n">
         <f aca="false">E273*(1+C274)</f>
         <v>8.46365488174945</v>
@@ -16623,6 +16896,7 @@
       <c r="C275" s="1" t="n">
         <v>0.046268</v>
       </c>
+      <c r="D275" s="1"/>
       <c r="E275" s="5" t="n">
         <f aca="false">E274*(1+C275)</f>
         <v>8.85525126581823</v>
@@ -16642,6 +16916,7 @@
       <c r="C276" s="1" t="n">
         <v>0.030817</v>
       </c>
+      <c r="D276" s="1"/>
       <c r="E276" s="5" t="n">
         <f aca="false">E275*(1+C276)</f>
         <v>9.12814354407695</v>
@@ -16661,6 +16936,7 @@
       <c r="C277" s="1" t="n">
         <v>0.02595</v>
       </c>
+      <c r="D277" s="1"/>
       <c r="E277" s="5" t="n">
         <f aca="false">E276*(1+C277)</f>
         <v>9.36501886904575</v>
@@ -16680,6 +16956,7 @@
       <c r="C278" s="1" t="n">
         <v>-0.034666</v>
       </c>
+      <c r="D278" s="1"/>
       <c r="E278" s="5" t="n">
         <f aca="false">E277*(1+C278)</f>
         <v>9.04037112493141</v>
@@ -16699,6 +16976,7 @@
       <c r="C279" s="1" t="n">
         <v>0.045757</v>
       </c>
+      <c r="D279" s="1"/>
       <c r="E279" s="5" t="n">
         <f aca="false">E278*(1+C279)</f>
         <v>9.45403138649489</v>
@@ -16718,6 +16996,7 @@
       <c r="C280" s="1" t="n">
         <v>0.008056</v>
       </c>
+      <c r="D280" s="1"/>
       <c r="E280" s="5" t="n">
         <f aca="false">E279*(1+C280)</f>
         <v>9.5301930633445</v>
@@ -16737,6 +17016,7 @@
       <c r="C281" s="1" t="n">
         <v>0.006555</v>
       </c>
+      <c r="D281" s="1"/>
       <c r="E281" s="5" t="n">
         <f aca="false">E280*(1+C281)</f>
         <v>9.59266347887472</v>
@@ -16756,6 +17036,7 @@
       <c r="C282" s="1" t="n">
         <v>0.023309</v>
       </c>
+      <c r="D282" s="1"/>
       <c r="E282" s="5" t="n">
         <f aca="false">E281*(1+C282)</f>
         <v>9.81625887190381</v>
@@ -16775,6 +17056,7 @@
       <c r="C283" s="1" t="n">
         <v>0.020635</v>
       </c>
+      <c r="D283" s="1"/>
       <c r="E283" s="5" t="n">
         <f aca="false">E282*(1+C283)</f>
         <v>10.0188173737255</v>
@@ -16794,6 +17076,7 @@
       <c r="C284" s="1" t="n">
         <v>-0.013974</v>
       </c>
+      <c r="D284" s="1"/>
       <c r="E284" s="5" t="n">
         <f aca="false">E283*(1+C284)</f>
         <v>9.87881441974511</v>
@@ -16813,6 +17096,7 @@
       <c r="C285" s="1" t="n">
         <v>0.039777</v>
       </c>
+      <c r="D285" s="1"/>
       <c r="E285" s="5" t="n">
         <f aca="false">E284*(1+C285)</f>
         <v>10.2717640209193</v>
@@ -16832,6 +17116,7 @@
       <c r="C286" s="1" t="n">
         <v>-0.013928</v>
       </c>
+      <c r="D286" s="1"/>
       <c r="E286" s="5" t="n">
         <f aca="false">E285*(1+C286)</f>
         <v>10.1286988916359</v>
@@ -16851,6 +17136,7 @@
       <c r="C287" s="1" t="n">
         <v>0.023972</v>
       </c>
+      <c r="D287" s="1"/>
       <c r="E287" s="5" t="n">
         <f aca="false">E286*(1+C287)</f>
         <v>10.3715040614662</v>
@@ -16870,6 +17156,7 @@
       <c r="C288" s="1" t="n">
         <v>0.027631</v>
       </c>
+      <c r="D288" s="1"/>
       <c r="E288" s="5" t="n">
         <f aca="false">E287*(1+C288)</f>
         <v>10.6580790901886</v>
@@ -16889,6 +17176,7 @@
       <c r="C289" s="1" t="n">
         <v>-0.002473</v>
       </c>
+      <c r="D289" s="1"/>
       <c r="E289" s="5" t="n">
         <f aca="false">E288*(1+C289)</f>
         <v>10.6317216605986</v>
@@ -16908,6 +17196,7 @@
       <c r="C290" s="1" t="n">
         <v>-0.02943</v>
       </c>
+      <c r="D290" s="1"/>
       <c r="E290" s="5" t="n">
         <f aca="false">E289*(1+C290)</f>
         <v>10.3188300921272</v>
@@ -16927,6 +17216,7 @@
       <c r="C291" s="1" t="n">
         <v>0.056976</v>
       </c>
+      <c r="D291" s="1"/>
       <c r="E291" s="5" t="n">
         <f aca="false">E290*(1+C291)</f>
         <v>10.9067557554562</v>
@@ -16946,6 +17236,7 @@
       <c r="C292" s="1" t="n">
         <v>-0.014993</v>
       </c>
+      <c r="D292" s="1"/>
       <c r="E292" s="5" t="n">
         <f aca="false">E291*(1+C292)</f>
         <v>10.7432307664146</v>
@@ -16965,6 +17256,7 @@
       <c r="C293" s="1" t="n">
         <v>0.009101</v>
       </c>
+      <c r="D293" s="1"/>
       <c r="E293" s="5" t="n">
         <f aca="false">E292*(1+C293)</f>
         <v>10.8410049096198</v>
@@ -16984,6 +17276,7 @@
       <c r="C294" s="1" t="n">
         <v>0.012522</v>
       </c>
+      <c r="D294" s="1"/>
       <c r="E294" s="5" t="n">
         <f aca="false">E293*(1+C294)</f>
         <v>10.976755973098</v>
@@ -17003,6 +17296,7 @@
       <c r="C295" s="1" t="n">
         <v>-0.019343</v>
       </c>
+      <c r="D295" s="1"/>
       <c r="E295" s="5" t="n">
         <f aca="false">E294*(1+C295)</f>
         <v>10.7644325823104</v>
@@ -17022,6 +17316,7 @@
       <c r="C296" s="1" t="n">
         <v>0.021297</v>
       </c>
+      <c r="D296" s="1"/>
       <c r="E296" s="5" t="n">
         <f aca="false">E295*(1+C296)</f>
         <v>10.9936827030159</v>
@@ -17041,6 +17336,7 @@
       <c r="C297" s="1" t="n">
         <v>-0.060073</v>
       </c>
+      <c r="D297" s="1"/>
       <c r="E297" s="5" t="n">
         <f aca="false">E296*(1+C297)</f>
         <v>10.3332592019976</v>
@@ -17060,6 +17356,7 @@
       <c r="C298" s="1" t="n">
         <v>-0.024548</v>
       </c>
+      <c r="D298" s="1"/>
       <c r="E298" s="5" t="n">
         <f aca="false">E297*(1+C298)</f>
         <v>10.079598355107</v>
@@ -17079,6 +17376,7 @@
       <c r="C299" s="1" t="n">
         <v>0.083449</v>
       </c>
+      <c r="D299" s="1"/>
       <c r="E299" s="5" t="n">
         <f aca="false">E298*(1+C299)</f>
         <v>10.9207307582423</v>
@@ -17098,6 +17396,7 @@
       <c r="C300" s="1" t="n">
         <v>0.003373</v>
       </c>
+      <c r="D300" s="1"/>
       <c r="E300" s="5" t="n">
         <f aca="false">E299*(1+C300)</f>
         <v>10.9575663830898</v>
@@ -17117,6 +17416,7 @@
       <c r="C301" s="1" t="n">
         <v>-0.015247</v>
       </c>
+      <c r="D301" s="1"/>
       <c r="E301" s="5" t="n">
         <f aca="false">E300*(1+C301)</f>
         <v>10.7904963684469</v>
@@ -17136,6 +17436,7 @@
       <c r="C302" s="1" t="n">
         <v>-0.0491</v>
       </c>
+      <c r="D302" s="1"/>
       <c r="E302" s="5" t="n">
         <f aca="false">E301*(1+C302)</f>
         <v>10.2606829967561</v>
@@ -17155,6 +17456,7 @@
       <c r="C303" s="1" t="n">
         <v>-0.001742</v>
       </c>
+      <c r="D303" s="1"/>
       <c r="E303" s="5" t="n">
         <f aca="false">E302*(1+C303)</f>
         <v>10.2428088869758</v>
@@ -17174,6 +17476,7 @@
       <c r="C304" s="1" t="n">
         <v>0.06734</v>
       </c>
+      <c r="D304" s="1"/>
       <c r="E304" s="5" t="n">
         <f aca="false">E303*(1+C304)</f>
         <v>10.9325596374247</v>
@@ -17193,6 +17496,7 @@
       <c r="C305" s="1" t="n">
         <v>0.003747</v>
       </c>
+      <c r="D305" s="1"/>
       <c r="E305" s="5" t="n">
         <f aca="false">E304*(1+C305)</f>
         <v>10.9735239383861</v>
@@ -17212,6 +17516,7 @@
       <c r="C306" s="1" t="n">
         <v>0.018487</v>
       </c>
+      <c r="D306" s="1"/>
       <c r="E306" s="5" t="n">
         <f aca="false">E305*(1+C306)</f>
         <v>11.1763914754351</v>
@@ -17231,6 +17536,7 @@
       <c r="C307" s="1" t="n">
         <v>0.002675</v>
       </c>
+      <c r="D307" s="1"/>
       <c r="E307" s="5" t="n">
         <f aca="false">E306*(1+C307)</f>
         <v>11.2062883226319</v>
@@ -17250,6 +17556,7 @@
       <c r="C308" s="1" t="n">
         <v>0.036571</v>
       </c>
+      <c r="D308" s="1"/>
       <c r="E308" s="5" t="n">
         <f aca="false">E307*(1+C308)</f>
         <v>11.6161134928789</v>
@@ -17269,6 +17576,7 @@
       <c r="C309" s="1" t="n">
         <v>0.001247</v>
       </c>
+      <c r="D309" s="1"/>
       <c r="E309" s="5" t="n">
         <f aca="false">E308*(1+C309)</f>
         <v>11.6305987864045</v>
@@ -17288,6 +17596,7 @@
       <c r="C310" s="1" t="n">
         <v>0.000446</v>
       </c>
+      <c r="D310" s="1"/>
       <c r="E310" s="5" t="n">
         <f aca="false">E309*(1+C310)</f>
         <v>11.6357860334632</v>
@@ -17307,6 +17616,7 @@
       <c r="C311" s="1" t="n">
         <v>-0.017944</v>
       </c>
+      <c r="D311" s="1"/>
       <c r="E311" s="5" t="n">
         <f aca="false">E310*(1+C311)</f>
         <v>11.4269934888787</v>
@@ -17326,6 +17636,7 @@
       <c r="C312" s="1" t="n">
         <v>0.035812</v>
       </c>
+      <c r="D312" s="1"/>
       <c r="E312" s="5" t="n">
         <f aca="false">E311*(1+C312)</f>
         <v>11.8362169797025</v>
@@ -17345,6 +17656,7 @@
       <c r="C313" s="1" t="n">
         <v>0.019204</v>
       </c>
+      <c r="D313" s="1"/>
       <c r="E313" s="5" t="n">
         <f aca="false">E312*(1+C313)</f>
         <v>12.0635196905807</v>
@@ -17364,6 +17676,7 @@
       <c r="C314" s="1" t="n">
         <v>0.019384</v>
       </c>
+      <c r="D314" s="1"/>
       <c r="E314" s="5" t="n">
         <f aca="false">E313*(1+C314)</f>
         <v>12.2973589562629</v>
@@ -17383,6 +17696,7 @@
       <c r="C315" s="1" t="n">
         <v>0.039459</v>
       </c>
+      <c r="D315" s="1"/>
       <c r="E315" s="5" t="n">
         <f aca="false">E314*(1+C315)</f>
         <v>12.7826004433181</v>
@@ -17402,6 +17716,7 @@
       <c r="C316" s="1" t="n">
         <v>0.001665</v>
       </c>
+      <c r="D316" s="1"/>
       <c r="E316" s="5" t="n">
         <f aca="false">E315*(1+C316)</f>
         <v>12.8038834730562</v>
@@ -17421,6 +17736,7 @@
       <c r="C317" s="1" t="n">
         <v>0.010591</v>
       </c>
+      <c r="D317" s="1"/>
       <c r="E317" s="5" t="n">
         <f aca="false">E316*(1+C317)</f>
         <v>12.9394894029193</v>
@@ -17440,6 +17756,7 @@
       <c r="C318" s="1" t="n">
         <v>0.014552</v>
       </c>
+      <c r="D318" s="1"/>
       <c r="E318" s="5" t="n">
         <f aca="false">E317*(1+C318)</f>
         <v>13.1277848527106</v>
@@ -17459,6 +17776,7 @@
       <c r="C319" s="1" t="n">
         <v>0.005798</v>
       </c>
+      <c r="D319" s="1"/>
       <c r="E319" s="5" t="n">
         <f aca="false">E318*(1+C319)</f>
         <v>13.2038997492866</v>
@@ -17478,6 +17796,7 @@
       <c r="C320" s="1" t="n">
         <v>0.020696</v>
       </c>
+      <c r="D320" s="1"/>
       <c r="E320" s="5" t="n">
         <f aca="false">E319*(1+C320)</f>
         <v>13.4771676584979</v>
@@ -17497,6 +17816,7 @@
       <c r="C321" s="1" t="n">
         <v>0.002238</v>
       </c>
+      <c r="D321" s="1"/>
       <c r="E321" s="5" t="n">
         <f aca="false">E320*(1+C321)</f>
         <v>13.5073295597176</v>
@@ -17516,6 +17836,7 @@
       <c r="C322" s="1" t="n">
         <v>0.02005</v>
       </c>
+      <c r="D322" s="1"/>
       <c r="E322" s="5" t="n">
         <f aca="false">E321*(1+C322)</f>
         <v>13.7781515173899</v>
@@ -17535,6 +17856,7 @@
       <c r="C323" s="1" t="n">
         <v>0.024132</v>
       </c>
+      <c r="D323" s="1"/>
       <c r="E323" s="5" t="n">
         <f aca="false">E322*(1+C323)</f>
         <v>14.1106458698076</v>
@@ -17554,6 +17876,7 @@
       <c r="C324" s="1" t="n">
         <v>0.031389</v>
       </c>
+      <c r="D324" s="1"/>
       <c r="E324" s="5" t="n">
         <f aca="false">E323*(1+C324)</f>
         <v>14.553564933015</v>
@@ -17573,6 +17896,7 @@
       <c r="C325" s="1" t="n">
         <v>0.011149</v>
       </c>
+      <c r="D325" s="1"/>
       <c r="E325" s="5" t="n">
         <f aca="false">E324*(1+C325)</f>
         <v>14.7158226284531</v>
@@ -17745,11 +18069,11 @@
   </sheetPr>
   <dimension ref="A1:L326"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="25.19"/>
@@ -17863,8 +18187,8 @@
         <v>14</v>
       </c>
       <c r="L4" s="1" t="n">
-        <f aca="false">STDEV(F3:F326)</f>
-        <v>0.0405412362716113</v>
+        <f aca="false">STDEV(E3:E326)</f>
+        <v>0.0405412362716111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26614,11 +26938,11 @@
   </sheetPr>
   <dimension ref="A1:L326"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="31.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="26.44"/>
@@ -26732,7 +27056,7 @@
         <v>14</v>
       </c>
       <c r="L4" s="1" t="n">
-        <f aca="false">STDEV(F3:F326)</f>
+        <f aca="false">STDEV(E3:E326)</f>
         <v>0.0463255415778035</v>
       </c>
     </row>

</xml_diff>